<commit_message>
translate languages and fix data
</commit_message>
<xml_diff>
--- a/docs/assets/language-file.xlsx
+++ b/docs/assets/language-file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas.gourouza/Documents/perso/langues/russian-voc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5BEF96-40D4-624A-9F64-2D27842069EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6C5DED-35EA-DC40-B066-7B171F47EFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="1260" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{B1898BFB-CE60-944F-9D77-C4636BC9C62B}"/>
+    <workbookView xWindow="5440" yWindow="1260" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{B1898BFB-CE60-944F-9D77-C4636BC9C62B}"/>
   </bookViews>
   <sheets>
     <sheet name="adjectives" sheetId="1" r:id="rId1"/>
@@ -6781,7 +6781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B40D6C6-14DC-254F-A6C4-6A36F011AECA}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
@@ -8178,8 +8178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EB28EE-E8CD-B544-9C3A-964FA168499D}">
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8633,11 +8633,11 @@
       <c r="B27" t="s">
         <v>165</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>216</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>217</v>
       </c>
       <c r="E27" s="30">
         <v>2</v>
@@ -8770,10 +8770,10 @@
         <v>165</v>
       </c>
       <c r="C35" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="D35" s="35" t="s">
         <v>171</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>230</v>
       </c>
       <c r="E35" s="30">
         <v>2</v>
@@ -8804,10 +8804,10 @@
         <v>165</v>
       </c>
       <c r="C37" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="35" t="s">
         <v>233</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>234</v>
       </c>
       <c r="E37" s="30">
         <v>2</v>
@@ -8889,10 +8889,10 @@
         <v>165</v>
       </c>
       <c r="C42" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="D42" s="36" t="s">
         <v>243</v>
-      </c>
-      <c r="D42" s="36" t="s">
-        <v>244</v>
       </c>
       <c r="E42" s="25">
         <v>3</v>
@@ -9986,7 +9986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="68">
+    <row r="107" spans="1:5" ht="85">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -19699,7 +19699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882F9811-2254-B74E-AA83-7675B912ED54}">
   <dimension ref="A1:E281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E281"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix language to lowercase
</commit_message>
<xml_diff>
--- a/docs/assets/language-file.xlsx
+++ b/docs/assets/language-file.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas.gourouza/Documents/perso/langues/russian-voc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6C5DED-35EA-DC40-B066-7B171F47EFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647FE96-2C38-034E-A2A0-EF79BE9F21AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="1260" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{B1898BFB-CE60-944F-9D77-C4636BC9C62B}"/>
+    <workbookView xWindow="5440" yWindow="1260" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{B1898BFB-CE60-944F-9D77-C4636BC9C62B}"/>
   </bookViews>
   <sheets>
-    <sheet name="adjectives" sheetId="1" r:id="rId1"/>
-    <sheet name="adverbs" sheetId="2" r:id="rId2"/>
-    <sheet name="conjunctions" sheetId="3" r:id="rId3"/>
-    <sheet name="expressions" sheetId="4" r:id="rId4"/>
-    <sheet name="nouns" sheetId="5" r:id="rId5"/>
-    <sheet name="verbs" sheetId="6" r:id="rId6"/>
+    <sheet name="Russian - Adjectives" sheetId="1" r:id="rId1"/>
+    <sheet name="Russian - Adverbs" sheetId="2" r:id="rId2"/>
+    <sheet name="Russian - Conjunctions" sheetId="3" r:id="rId3"/>
+    <sheet name="Russian - Expressions" sheetId="4" r:id="rId4"/>
+    <sheet name="Russian - Nouns" sheetId="5" r:id="rId5"/>
+    <sheet name="Russian - Verbs" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -8178,7 +8178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EB28EE-E8CD-B544-9C3A-964FA168499D}">
   <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -10846,8 +10846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDDFAEA-4718-6141-8AD3-3399454A9EC9}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19700,7 +19700,7 @@
   <dimension ref="A1:E281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E281"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24484,5 +24484,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>